<commit_message>
added test and test data for endoduplication
</commit_message>
<xml_diff>
--- a/TEST-DATA-SETS.xlsx
+++ b/TEST-DATA-SETS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brennalevine/Desktop/ParthenoGenius/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{444CA007-D647-BD40-97A5-44D2F3C5F7E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5727E997-25E0-384A-9990-BC56DB468433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16280" activeTab="1" xr2:uid="{03B7548E-D43F-6D4B-A254-868072420310}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16280" activeTab="2" xr2:uid="{03B7548E-D43F-6D4B-A254-868072420310}"/>
   </bookViews>
   <sheets>
     <sheet name="NON-PARTH" sheetId="6" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
     <sheet name="TERM-FUS" sheetId="2" r:id="rId5"/>
     <sheet name="GAM-DUP" sheetId="1" r:id="rId6"/>
+    <sheet name="ENDO-DUP" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="119">
   <si>
     <t>SNP_1</t>
   </si>
@@ -395,6 +396,9 @@
   </si>
   <si>
     <t>Baby has heterozygosity at 10 of mom's homozygous alleles</t>
+  </si>
+  <si>
+    <t>Retained heterozygogosity at 63 loci</t>
   </si>
 </sst>
 </file>
@@ -2543,7 +2547,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBFA3464-96A8-6A4A-81AA-BFA699F17C02}">
   <dimension ref="A1:CW5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
@@ -4080,7 +4084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A6C0DE-52C1-504E-8460-C299711FCE7A}">
   <dimension ref="A1:CW48"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="K26" sqref="K26:K27"/>
     </sheetView>
   </sheetViews>
@@ -11396,4 +11400,1807 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2825010-244E-9A4E-BC46-BC72447BD7EC}">
+  <dimension ref="A1:CW48"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>67</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>69</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>70</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BY1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>76</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>77</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>78</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>79</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>80</v>
+      </c>
+      <c r="CE1" t="s">
+        <v>81</v>
+      </c>
+      <c r="CF1" t="s">
+        <v>82</v>
+      </c>
+      <c r="CG1" t="s">
+        <v>83</v>
+      </c>
+      <c r="CH1" t="s">
+        <v>84</v>
+      </c>
+      <c r="CI1" t="s">
+        <v>85</v>
+      </c>
+      <c r="CJ1" t="s">
+        <v>86</v>
+      </c>
+      <c r="CK1" t="s">
+        <v>87</v>
+      </c>
+      <c r="CL1" t="s">
+        <v>88</v>
+      </c>
+      <c r="CM1" t="s">
+        <v>89</v>
+      </c>
+      <c r="CN1" t="s">
+        <v>90</v>
+      </c>
+      <c r="CO1" t="s">
+        <v>91</v>
+      </c>
+      <c r="CP1" t="s">
+        <v>92</v>
+      </c>
+      <c r="CQ1" t="s">
+        <v>93</v>
+      </c>
+      <c r="CR1" t="s">
+        <v>94</v>
+      </c>
+      <c r="CS1" t="s">
+        <v>95</v>
+      </c>
+      <c r="CT1" t="s">
+        <v>96</v>
+      </c>
+      <c r="CU1" t="s">
+        <v>97</v>
+      </c>
+      <c r="CV1" t="s">
+        <v>98</v>
+      </c>
+      <c r="CW1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2" s="2">
+        <v>-9</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2" s="1">
+        <v>1</v>
+      </c>
+      <c r="T2" s="1">
+        <v>1</v>
+      </c>
+      <c r="U2" s="1">
+        <v>0</v>
+      </c>
+      <c r="V2" s="1">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>0</v>
+      </c>
+      <c r="AK2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN2" s="2">
+        <v>-9</v>
+      </c>
+      <c r="AO2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP2">
+        <v>0</v>
+      </c>
+      <c r="AQ2">
+        <v>0</v>
+      </c>
+      <c r="AR2">
+        <v>0</v>
+      </c>
+      <c r="AS2">
+        <v>0</v>
+      </c>
+      <c r="AT2">
+        <v>0</v>
+      </c>
+      <c r="AU2">
+        <v>1</v>
+      </c>
+      <c r="AV2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AW2">
+        <v>0</v>
+      </c>
+      <c r="AX2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ2">
+        <v>1</v>
+      </c>
+      <c r="BA2">
+        <v>0</v>
+      </c>
+      <c r="BB2">
+        <v>0</v>
+      </c>
+      <c r="BC2" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BE2">
+        <v>0</v>
+      </c>
+      <c r="BF2">
+        <v>0</v>
+      </c>
+      <c r="BG2">
+        <v>0</v>
+      </c>
+      <c r="BH2">
+        <v>0</v>
+      </c>
+      <c r="BI2">
+        <v>0</v>
+      </c>
+      <c r="BJ2">
+        <v>0</v>
+      </c>
+      <c r="BK2">
+        <v>0</v>
+      </c>
+      <c r="BL2">
+        <v>0</v>
+      </c>
+      <c r="BM2" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN2">
+        <v>0</v>
+      </c>
+      <c r="BO2">
+        <v>0</v>
+      </c>
+      <c r="BP2">
+        <v>0</v>
+      </c>
+      <c r="BQ2">
+        <v>0</v>
+      </c>
+      <c r="BR2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BS2" s="1">
+        <v>0</v>
+      </c>
+      <c r="BT2" s="1">
+        <v>0</v>
+      </c>
+      <c r="BU2">
+        <v>0</v>
+      </c>
+      <c r="BV2">
+        <v>0</v>
+      </c>
+      <c r="BW2">
+        <v>0</v>
+      </c>
+      <c r="BX2">
+        <v>0</v>
+      </c>
+      <c r="BY2">
+        <v>0</v>
+      </c>
+      <c r="BZ2">
+        <v>0</v>
+      </c>
+      <c r="CA2">
+        <v>0</v>
+      </c>
+      <c r="CB2" s="1">
+        <v>1</v>
+      </c>
+      <c r="CC2" s="1">
+        <v>0</v>
+      </c>
+      <c r="CD2">
+        <v>0</v>
+      </c>
+      <c r="CE2">
+        <v>0</v>
+      </c>
+      <c r="CF2">
+        <v>0</v>
+      </c>
+      <c r="CG2">
+        <v>0</v>
+      </c>
+      <c r="CH2">
+        <v>0</v>
+      </c>
+      <c r="CI2">
+        <v>0</v>
+      </c>
+      <c r="CJ2">
+        <v>0</v>
+      </c>
+      <c r="CK2">
+        <v>0</v>
+      </c>
+      <c r="CL2">
+        <v>0</v>
+      </c>
+      <c r="CM2" s="1">
+        <v>0</v>
+      </c>
+      <c r="CN2" s="1">
+        <v>0</v>
+      </c>
+      <c r="CO2" s="1">
+        <v>1</v>
+      </c>
+      <c r="CP2" s="1">
+        <v>1</v>
+      </c>
+      <c r="CQ2" s="1">
+        <v>0</v>
+      </c>
+      <c r="CR2">
+        <v>0</v>
+      </c>
+      <c r="CS2">
+        <v>0</v>
+      </c>
+      <c r="CT2">
+        <v>0</v>
+      </c>
+      <c r="CU2">
+        <v>0</v>
+      </c>
+      <c r="CV2">
+        <v>0</v>
+      </c>
+      <c r="CW2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2">
+        <v>-9</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3" s="1">
+        <v>1</v>
+      </c>
+      <c r="T3" s="1">
+        <v>1</v>
+      </c>
+      <c r="U3" s="1">
+        <v>0</v>
+      </c>
+      <c r="V3" s="1">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>1</v>
+      </c>
+      <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AB3">
+        <v>1</v>
+      </c>
+      <c r="AC3">
+        <v>1</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <v>1</v>
+      </c>
+      <c r="AH3">
+        <v>1</v>
+      </c>
+      <c r="AI3">
+        <v>1</v>
+      </c>
+      <c r="AJ3">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN3" s="2">
+        <v>-9</v>
+      </c>
+      <c r="AO3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP3">
+        <v>1</v>
+      </c>
+      <c r="AQ3">
+        <v>1</v>
+      </c>
+      <c r="AR3">
+        <v>1</v>
+      </c>
+      <c r="AS3">
+        <v>1</v>
+      </c>
+      <c r="AT3">
+        <v>1</v>
+      </c>
+      <c r="AU3">
+        <v>0</v>
+      </c>
+      <c r="AV3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AW3">
+        <v>1</v>
+      </c>
+      <c r="AX3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ3">
+        <v>0</v>
+      </c>
+      <c r="BA3">
+        <v>1</v>
+      </c>
+      <c r="BB3">
+        <v>1</v>
+      </c>
+      <c r="BC3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD3" s="1">
+        <v>1</v>
+      </c>
+      <c r="BE3">
+        <v>1</v>
+      </c>
+      <c r="BF3">
+        <v>1</v>
+      </c>
+      <c r="BG3">
+        <v>1</v>
+      </c>
+      <c r="BH3">
+        <v>1</v>
+      </c>
+      <c r="BI3">
+        <v>1</v>
+      </c>
+      <c r="BJ3">
+        <v>1</v>
+      </c>
+      <c r="BK3">
+        <v>1</v>
+      </c>
+      <c r="BL3">
+        <v>1</v>
+      </c>
+      <c r="BM3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN3">
+        <v>1</v>
+      </c>
+      <c r="BO3">
+        <v>1</v>
+      </c>
+      <c r="BP3">
+        <v>1</v>
+      </c>
+      <c r="BQ3">
+        <v>1</v>
+      </c>
+      <c r="BR3" s="1">
+        <v>1</v>
+      </c>
+      <c r="BS3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BT3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BU3">
+        <v>1</v>
+      </c>
+      <c r="BV3">
+        <v>1</v>
+      </c>
+      <c r="BW3">
+        <v>1</v>
+      </c>
+      <c r="BX3">
+        <v>1</v>
+      </c>
+      <c r="BY3">
+        <v>1</v>
+      </c>
+      <c r="BZ3">
+        <v>1</v>
+      </c>
+      <c r="CA3">
+        <v>1</v>
+      </c>
+      <c r="CB3" s="1">
+        <v>1</v>
+      </c>
+      <c r="CC3" s="1">
+        <v>0</v>
+      </c>
+      <c r="CD3">
+        <v>1</v>
+      </c>
+      <c r="CE3">
+        <v>1</v>
+      </c>
+      <c r="CF3">
+        <v>1</v>
+      </c>
+      <c r="CG3">
+        <v>1</v>
+      </c>
+      <c r="CH3">
+        <v>1</v>
+      </c>
+      <c r="CI3">
+        <v>1</v>
+      </c>
+      <c r="CJ3">
+        <v>1</v>
+      </c>
+      <c r="CK3">
+        <v>1</v>
+      </c>
+      <c r="CL3">
+        <v>1</v>
+      </c>
+      <c r="CM3" s="1">
+        <v>0</v>
+      </c>
+      <c r="CN3" s="1">
+        <v>0</v>
+      </c>
+      <c r="CO3" s="1">
+        <v>1</v>
+      </c>
+      <c r="CP3" s="1">
+        <v>1</v>
+      </c>
+      <c r="CQ3" s="1">
+        <v>0</v>
+      </c>
+      <c r="CR3">
+        <v>1</v>
+      </c>
+      <c r="CS3">
+        <v>1</v>
+      </c>
+      <c r="CT3">
+        <v>1</v>
+      </c>
+      <c r="CU3">
+        <v>1</v>
+      </c>
+      <c r="CV3">
+        <v>1</v>
+      </c>
+      <c r="CW3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="3">
+        <v>1</v>
+      </c>
+      <c r="M4" s="3">
+        <v>1</v>
+      </c>
+      <c r="N4" s="3">
+        <v>1</v>
+      </c>
+      <c r="O4" s="3">
+        <v>0</v>
+      </c>
+      <c r="P4" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>0</v>
+      </c>
+      <c r="R4" s="3">
+        <v>1</v>
+      </c>
+      <c r="S4" s="1">
+        <v>1</v>
+      </c>
+      <c r="T4" s="1">
+        <v>1</v>
+      </c>
+      <c r="U4" s="1">
+        <v>0</v>
+      </c>
+      <c r="V4" s="1">
+        <v>0</v>
+      </c>
+      <c r="W4" s="3">
+        <v>0</v>
+      </c>
+      <c r="X4" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="3">
+        <v>1</v>
+      </c>
+      <c r="AJ4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN4">
+        <v>1</v>
+      </c>
+      <c r="AO4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AQ4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AR4" s="3">
+        <v>1</v>
+      </c>
+      <c r="AS4" s="3">
+        <v>1</v>
+      </c>
+      <c r="AT4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AU4" s="3">
+        <v>1</v>
+      </c>
+      <c r="AV4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AW4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AX4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY4" s="2">
+        <v>-9</v>
+      </c>
+      <c r="AZ4" s="3">
+        <v>1</v>
+      </c>
+      <c r="BA4" s="3">
+        <v>1</v>
+      </c>
+      <c r="BB4" s="3">
+        <v>0</v>
+      </c>
+      <c r="BC4" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD4" s="1">
+        <v>1</v>
+      </c>
+      <c r="BE4" s="3">
+        <v>1</v>
+      </c>
+      <c r="BF4" s="3">
+        <v>0</v>
+      </c>
+      <c r="BG4" s="3">
+        <v>0</v>
+      </c>
+      <c r="BH4" s="3">
+        <v>0</v>
+      </c>
+      <c r="BI4" s="3">
+        <v>0</v>
+      </c>
+      <c r="BJ4" s="3">
+        <v>1</v>
+      </c>
+      <c r="BK4" s="3">
+        <v>0</v>
+      </c>
+      <c r="BL4" s="3">
+        <v>0</v>
+      </c>
+      <c r="BM4" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN4" s="3">
+        <v>0</v>
+      </c>
+      <c r="BO4" s="3">
+        <v>0</v>
+      </c>
+      <c r="BP4" s="3">
+        <v>1</v>
+      </c>
+      <c r="BQ4" s="3">
+        <v>1</v>
+      </c>
+      <c r="BR4" s="1">
+        <v>1</v>
+      </c>
+      <c r="BS4" s="1">
+        <v>0</v>
+      </c>
+      <c r="BT4" s="1">
+        <v>0</v>
+      </c>
+      <c r="BU4" s="3">
+        <v>0</v>
+      </c>
+      <c r="BV4" s="3">
+        <v>0</v>
+      </c>
+      <c r="BW4" s="3">
+        <v>0</v>
+      </c>
+      <c r="BX4" s="3">
+        <v>0</v>
+      </c>
+      <c r="BY4" s="3">
+        <v>1</v>
+      </c>
+      <c r="BZ4" s="3">
+        <v>0</v>
+      </c>
+      <c r="CA4" s="3">
+        <v>1</v>
+      </c>
+      <c r="CB4" s="1">
+        <v>1</v>
+      </c>
+      <c r="CC4" s="1">
+        <v>0</v>
+      </c>
+      <c r="CD4" s="3">
+        <v>0</v>
+      </c>
+      <c r="CE4" s="3">
+        <v>1</v>
+      </c>
+      <c r="CF4" s="3">
+        <v>1</v>
+      </c>
+      <c r="CG4" s="3">
+        <v>1</v>
+      </c>
+      <c r="CH4" s="3">
+        <v>0</v>
+      </c>
+      <c r="CI4" s="3">
+        <v>0</v>
+      </c>
+      <c r="CJ4" s="3">
+        <v>0</v>
+      </c>
+      <c r="CK4" s="3">
+        <v>0</v>
+      </c>
+      <c r="CL4" s="3">
+        <v>0</v>
+      </c>
+      <c r="CM4" s="1">
+        <v>0</v>
+      </c>
+      <c r="CN4" s="1">
+        <v>0</v>
+      </c>
+      <c r="CO4" s="1">
+        <v>1</v>
+      </c>
+      <c r="CP4" s="1">
+        <v>1</v>
+      </c>
+      <c r="CQ4" s="1">
+        <v>0</v>
+      </c>
+      <c r="CR4" s="3">
+        <v>0</v>
+      </c>
+      <c r="CS4" s="3">
+        <v>0</v>
+      </c>
+      <c r="CT4" s="3">
+        <v>0</v>
+      </c>
+      <c r="CU4" s="3">
+        <v>0</v>
+      </c>
+      <c r="CV4" s="3">
+        <v>0</v>
+      </c>
+      <c r="CW4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="2">
+        <v>-9</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="3">
+        <v>0</v>
+      </c>
+      <c r="M5" s="3">
+        <v>0</v>
+      </c>
+      <c r="N5" s="3">
+        <v>0</v>
+      </c>
+      <c r="O5" s="3">
+        <v>1</v>
+      </c>
+      <c r="P5" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>1</v>
+      </c>
+      <c r="R5" s="3">
+        <v>0</v>
+      </c>
+      <c r="S5" s="1">
+        <v>1</v>
+      </c>
+      <c r="T5" s="1">
+        <v>1</v>
+      </c>
+      <c r="U5" s="1">
+        <v>0</v>
+      </c>
+      <c r="V5" s="1">
+        <v>0</v>
+      </c>
+      <c r="W5" s="3">
+        <v>1</v>
+      </c>
+      <c r="X5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AH5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AI5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AK5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN5">
+        <v>1</v>
+      </c>
+      <c r="AO5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AQ5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AR5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AS5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AT5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AU5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AV5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AW5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AX5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ5" s="3">
+        <v>0</v>
+      </c>
+      <c r="BA5" s="3">
+        <v>0</v>
+      </c>
+      <c r="BB5" s="3">
+        <v>1</v>
+      </c>
+      <c r="BC5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD5" s="1">
+        <v>1</v>
+      </c>
+      <c r="BE5" s="3">
+        <v>0</v>
+      </c>
+      <c r="BF5" s="3">
+        <v>1</v>
+      </c>
+      <c r="BG5" s="3">
+        <v>1</v>
+      </c>
+      <c r="BH5" s="3">
+        <v>1</v>
+      </c>
+      <c r="BI5" s="3">
+        <v>1</v>
+      </c>
+      <c r="BJ5" s="3">
+        <v>0</v>
+      </c>
+      <c r="BK5" s="3">
+        <v>1</v>
+      </c>
+      <c r="BL5" s="3">
+        <v>1</v>
+      </c>
+      <c r="BM5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN5" s="3">
+        <v>1</v>
+      </c>
+      <c r="BO5" s="3">
+        <v>1</v>
+      </c>
+      <c r="BP5" s="3">
+        <v>0</v>
+      </c>
+      <c r="BQ5" s="3">
+        <v>0</v>
+      </c>
+      <c r="BR5" s="1">
+        <v>1</v>
+      </c>
+      <c r="BS5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BT5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BU5" s="3">
+        <v>1</v>
+      </c>
+      <c r="BV5" s="3">
+        <v>1</v>
+      </c>
+      <c r="BW5" s="3">
+        <v>1</v>
+      </c>
+      <c r="BX5" s="3">
+        <v>1</v>
+      </c>
+      <c r="BY5" s="3">
+        <v>0</v>
+      </c>
+      <c r="BZ5" s="3">
+        <v>1</v>
+      </c>
+      <c r="CA5" s="3">
+        <v>0</v>
+      </c>
+      <c r="CB5" s="1">
+        <v>1</v>
+      </c>
+      <c r="CC5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CD5" s="3">
+        <v>1</v>
+      </c>
+      <c r="CE5" s="3">
+        <v>0</v>
+      </c>
+      <c r="CF5" s="3">
+        <v>0</v>
+      </c>
+      <c r="CG5" s="3">
+        <v>0</v>
+      </c>
+      <c r="CH5" s="3">
+        <v>1</v>
+      </c>
+      <c r="CI5" s="3">
+        <v>1</v>
+      </c>
+      <c r="CJ5" s="3">
+        <v>1</v>
+      </c>
+      <c r="CK5" s="3">
+        <v>1</v>
+      </c>
+      <c r="CL5" s="3">
+        <v>1</v>
+      </c>
+      <c r="CM5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CN5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CO5" s="1">
+        <v>1</v>
+      </c>
+      <c r="CP5" s="1">
+        <v>1</v>
+      </c>
+      <c r="CQ5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CR5" s="3">
+        <v>1</v>
+      </c>
+      <c r="CS5" s="3">
+        <v>1</v>
+      </c>
+      <c r="CT5" s="3">
+        <v>1</v>
+      </c>
+      <c r="CU5" s="3">
+        <v>1</v>
+      </c>
+      <c r="CV5" s="3">
+        <v>1</v>
+      </c>
+      <c r="CW5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E7" t="s">
+        <v>110</v>
+      </c>
+      <c r="H7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>